<commit_message>
MDPs terminados con v3 que puede ser mejor que la v2
</commit_message>
<xml_diff>
--- a/catkin_ws/src/icra2024/src/MDPs/policy_left_lane.xlsx
+++ b/catkin_ws/src/icra2024/src/MDPs/policy_left_lane.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="17">
   <si>
     <t xml:space="preserve">Polìtica original V1</t>
   </si>
@@ -52,10 +52,10 @@
     <t xml:space="preserve"> free_NE(0)=1</t>
   </si>
   <si>
-    <t xml:space="preserve"> sE1(0)=1</t>
+    <t xml:space="preserve"> sE2(0)=0) = change_lane</t>
   </si>
   <si>
-    <t xml:space="preserve"> sE2(0)=0) = change_lane</t>
+    <t xml:space="preserve"> sE1(0)=1</t>
   </si>
   <si>
     <t xml:space="preserve">change_lane</t>
@@ -202,16 +202,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:T68"/>
+  <dimension ref="A1:AA68"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L25" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P3" activeCellId="0" sqref="P3:U34"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="S13" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="W3" activeCellId="0" sqref="W3:AB34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="1.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="17.56"/>
@@ -269,6 +269,21 @@
       <c r="T3" s="0" t="s">
         <v>5</v>
       </c>
+      <c r="W3" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="X3" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y3" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z3" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA3" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
@@ -316,6 +331,21 @@
       <c r="T4" s="0" t="s">
         <v>5</v>
       </c>
+      <c r="W4" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="X4" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y4" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z4" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA4" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
@@ -363,6 +393,21 @@
       <c r="T5" s="0" t="s">
         <v>8</v>
       </c>
+      <c r="W5" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="X5" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y5" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z5" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA5" s="0" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
@@ -410,6 +455,21 @@
       <c r="T6" s="0" t="s">
         <v>8</v>
       </c>
+      <c r="W6" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="X6" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y6" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z6" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA6" s="0" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
@@ -457,6 +517,21 @@
       <c r="T7" s="0" t="s">
         <v>5</v>
       </c>
+      <c r="W7" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="X7" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y7" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z7" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA7" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
@@ -504,6 +579,21 @@
       <c r="T8" s="0" t="s">
         <v>5</v>
       </c>
+      <c r="W8" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="X8" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y8" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z8" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA8" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
@@ -551,6 +641,21 @@
       <c r="T9" s="0" t="s">
         <v>8</v>
       </c>
+      <c r="W9" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="X9" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y9" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z9" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA9" s="0" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
@@ -598,6 +703,21 @@
       <c r="T10" s="0" t="s">
         <v>8</v>
       </c>
+      <c r="W10" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="X10" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y10" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z10" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA10" s="0" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
@@ -610,7 +730,7 @@
         <v>3</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>5</v>
@@ -625,7 +745,7 @@
         <v>3</v>
       </c>
       <c r="L11" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M11" s="0" t="s">
         <v>5</v>
@@ -640,9 +760,24 @@
         <v>3</v>
       </c>
       <c r="S11" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="T11" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="W11" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="X11" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y11" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z11" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA11" s="0" t="s">
         <v>5</v>
       </c>
     </row>
@@ -657,7 +792,7 @@
         <v>3</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>5</v>
@@ -672,7 +807,7 @@
         <v>3</v>
       </c>
       <c r="L12" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M12" s="0" t="s">
         <v>5</v>
@@ -687,9 +822,24 @@
         <v>3</v>
       </c>
       <c r="S12" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="T12" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="W12" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="X12" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y12" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z12" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA12" s="0" t="s">
         <v>5</v>
       </c>
     </row>
@@ -704,7 +854,7 @@
         <v>3</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>8</v>
@@ -719,7 +869,7 @@
         <v>3</v>
       </c>
       <c r="L13" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M13" s="0" t="s">
         <v>8</v>
@@ -734,9 +884,24 @@
         <v>3</v>
       </c>
       <c r="S13" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="T13" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="W13" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="X13" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y13" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z13" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA13" s="0" t="s">
         <v>8</v>
       </c>
     </row>
@@ -751,7 +916,7 @@
         <v>3</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>8</v>
@@ -766,7 +931,7 @@
         <v>3</v>
       </c>
       <c r="L14" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M14" s="0" t="s">
         <v>8</v>
@@ -781,9 +946,24 @@
         <v>3</v>
       </c>
       <c r="S14" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="T14" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="W14" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="X14" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y14" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z14" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA14" s="0" t="s">
         <v>8</v>
       </c>
     </row>
@@ -798,7 +978,7 @@
         <v>9</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>5</v>
@@ -813,7 +993,7 @@
         <v>9</v>
       </c>
       <c r="L15" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M15" s="0" t="s">
         <v>5</v>
@@ -828,9 +1008,24 @@
         <v>9</v>
       </c>
       <c r="S15" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="T15" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="W15" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="X15" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y15" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z15" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA15" s="0" t="s">
         <v>5</v>
       </c>
     </row>
@@ -845,11 +1040,11 @@
         <v>9</v>
       </c>
       <c r="D16" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E16" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="I16" s="4" t="s">
         <v>6</v>
       </c>
@@ -860,11 +1055,11 @@
         <v>9</v>
       </c>
       <c r="L16" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="M16" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="M16" s="4" t="s">
-        <v>11</v>
-      </c>
       <c r="P16" s="4" t="s">
         <v>6</v>
       </c>
@@ -875,10 +1070,25 @@
         <v>9</v>
       </c>
       <c r="S16" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="T16" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="T16" s="4" t="s">
-        <v>11</v>
+      <c r="W16" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="X16" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y16" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z16" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA16" s="4" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -892,7 +1102,7 @@
         <v>9</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>8</v>
@@ -907,7 +1117,7 @@
         <v>9</v>
       </c>
       <c r="L17" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M17" s="0" t="s">
         <v>8</v>
@@ -922,9 +1132,24 @@
         <v>9</v>
       </c>
       <c r="S17" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="T17" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="W17" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="X17" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y17" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z17" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA17" s="0" t="s">
         <v>8</v>
       </c>
     </row>
@@ -939,7 +1164,7 @@
         <v>9</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>8</v>
@@ -957,11 +1182,11 @@
         <v>9</v>
       </c>
       <c r="L18" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="M18" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="M18" s="4" t="s">
-        <v>11</v>
-      </c>
       <c r="P18" s="4" t="s">
         <v>6</v>
       </c>
@@ -972,10 +1197,25 @@
         <v>9</v>
       </c>
       <c r="S18" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="T18" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="T18" s="4" t="s">
-        <v>11</v>
+      <c r="W18" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="X18" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y18" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z18" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA18" s="4" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1024,6 +1264,21 @@
       <c r="T19" s="0" t="s">
         <v>13</v>
       </c>
+      <c r="W19" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="X19" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y19" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z19" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA19" s="0" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
@@ -1071,6 +1326,21 @@
       <c r="T20" s="0" t="s">
         <v>13</v>
       </c>
+      <c r="W20" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="X20" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y20" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z20" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA20" s="0" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
@@ -1118,6 +1388,21 @@
       <c r="T21" s="0" t="s">
         <v>14</v>
       </c>
+      <c r="W21" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="X21" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y21" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z21" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA21" s="0" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
@@ -1165,6 +1450,21 @@
       <c r="T22" s="0" t="s">
         <v>14</v>
       </c>
+      <c r="W22" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="X22" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y22" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z22" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA22" s="0" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
@@ -1212,6 +1512,21 @@
       <c r="T23" s="0" t="s">
         <v>13</v>
       </c>
+      <c r="W23" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="X23" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y23" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z23" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA23" s="0" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="24" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="3" t="s">
@@ -1259,6 +1574,21 @@
       <c r="T24" s="4" t="s">
         <v>15</v>
       </c>
+      <c r="W24" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="X24" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y24" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z24" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA24" s="4" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
@@ -1306,6 +1636,21 @@
       <c r="T25" s="0" t="s">
         <v>14</v>
       </c>
+      <c r="W25" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="X25" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y25" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z25" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA25" s="0" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="26" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="3" t="s">
@@ -1356,6 +1701,21 @@
       <c r="T26" s="4" t="s">
         <v>15</v>
       </c>
+      <c r="W26" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="X26" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y26" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z26" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA26" s="4" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
@@ -1368,7 +1728,7 @@
         <v>3</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>13</v>
@@ -1383,7 +1743,7 @@
         <v>3</v>
       </c>
       <c r="L27" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M27" s="0" t="s">
         <v>13</v>
@@ -1398,9 +1758,24 @@
         <v>3</v>
       </c>
       <c r="S27" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="T27" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="W27" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="X27" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y27" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z27" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA27" s="0" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1415,7 +1790,7 @@
         <v>3</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>13</v>
@@ -1430,7 +1805,7 @@
         <v>3</v>
       </c>
       <c r="L28" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M28" s="0" t="s">
         <v>13</v>
@@ -1445,9 +1820,24 @@
         <v>3</v>
       </c>
       <c r="S28" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="T28" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="W28" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="X28" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y28" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z28" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA28" s="0" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1462,7 +1852,7 @@
         <v>3</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>14</v>
@@ -1477,7 +1867,7 @@
         <v>3</v>
       </c>
       <c r="L29" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M29" s="0" t="s">
         <v>14</v>
@@ -1492,9 +1882,24 @@
         <v>3</v>
       </c>
       <c r="S29" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="T29" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="W29" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="X29" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y29" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z29" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA29" s="0" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1509,7 +1914,7 @@
         <v>3</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>14</v>
@@ -1524,7 +1929,7 @@
         <v>3</v>
       </c>
       <c r="L30" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M30" s="0" t="s">
         <v>14</v>
@@ -1539,9 +1944,24 @@
         <v>3</v>
       </c>
       <c r="S30" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="T30" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="W30" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="X30" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y30" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z30" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA30" s="0" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1556,7 +1976,7 @@
         <v>9</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>13</v>
@@ -1571,7 +1991,7 @@
         <v>9</v>
       </c>
       <c r="L31" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M31" s="0" t="s">
         <v>13</v>
@@ -1586,9 +2006,24 @@
         <v>9</v>
       </c>
       <c r="S31" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="T31" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="W31" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="X31" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y31" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z31" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA31" s="0" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1603,7 +2038,7 @@
         <v>9</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>15</v>
@@ -1618,7 +2053,7 @@
         <v>9</v>
       </c>
       <c r="L32" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M32" s="4" t="s">
         <v>15</v>
@@ -1633,11 +2068,26 @@
         <v>9</v>
       </c>
       <c r="S32" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="T32" s="4" t="s">
         <v>15</v>
       </c>
+      <c r="W32" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="X32" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y32" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z32" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA32" s="4" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
@@ -1650,7 +2100,7 @@
         <v>9</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>14</v>
@@ -1665,7 +2115,7 @@
         <v>9</v>
       </c>
       <c r="L33" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M33" s="0" t="s">
         <v>14</v>
@@ -1680,9 +2130,24 @@
         <v>9</v>
       </c>
       <c r="S33" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="T33" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="W33" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="X33" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y33" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z33" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA33" s="0" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1697,7 +2162,7 @@
         <v>9</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E34" s="3" t="s">
         <v>14</v>
@@ -1715,7 +2180,7 @@
         <v>9</v>
       </c>
       <c r="L34" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M34" s="4" t="s">
         <v>15</v>
@@ -1730,9 +2195,24 @@
         <v>9</v>
       </c>
       <c r="S34" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="T34" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="W34" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="X34" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y34" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z34" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA34" s="4" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Cambio de política de 32 a 16 estados en cada carril
</commit_message>
<xml_diff>
--- a/catkin_ws/src/icra2024/src/MDPs/policy_left_lane.xlsx
+++ b/catkin_ws/src/icra2024/src/MDPs/policy_left_lane.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="32" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="16" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="774" uniqueCount="24">
   <si>
     <t xml:space="preserve">Polìtica original V1</t>
   </si>
@@ -75,6 +76,27 @@
 0  1  SW car has equal speed
 0  0  SW car has faster speed</t>
   </si>
+  <si>
+    <t xml:space="preserve"> free_SE(0)=0) = keep_distance</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> free_SE(0)=0) = cruise</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> free_SE(0)=0) = change_lane</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aquí se supone que los carros de la derecha vienen más lento y hay chance de cambiar de carril</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> free_SE(0)=1) = keep_distance</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> free_SE(0)=1) = cruise</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> free_SE(0)=1) = change_lane</t>
+  </si>
 </sst>
 </file>
 
@@ -83,7 +105,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -104,6 +126,12 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="22"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -160,7 +188,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -185,6 +213,18 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -204,11 +244,11 @@
   </sheetPr>
   <dimension ref="A1:AA68"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="S13" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="W3" activeCellId="0" sqref="W3:AB34"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="S1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="W3" activeCellId="0" sqref="W3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.98"/>
@@ -2233,4 +2273,475 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A2:AMJ17"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="71" zoomScaleNormal="71" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="31.1484375" defaultRowHeight="26.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="6" width="39.72"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="2" style="6" width="31.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="6" width="37.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="6" width="25.63"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1020" min="11" style="6" width="31.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1021" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="2" customFormat="false" ht="26.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="26.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="26.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="L4" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="26.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="K5" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="L5" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="26.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="7"/>
+      <c r="I6" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="K6" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="L6" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" s="8" customFormat="true" ht="26.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="I7" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="J7" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="K7" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="L7" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="AMG7" s="4"/>
+      <c r="AMH7" s="4"/>
+      <c r="AMI7" s="4"/>
+      <c r="AMJ7" s="4"/>
+    </row>
+    <row r="8" customFormat="false" ht="26.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="7"/>
+      <c r="I8" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="J8" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="K8" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="L8" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" s="8" customFormat="true" ht="26.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="I9" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="J9" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="K9" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="L9" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="AMG9" s="4"/>
+      <c r="AMH9" s="4"/>
+      <c r="AMI9" s="4"/>
+      <c r="AMJ9" s="4"/>
+    </row>
+    <row r="10" customFormat="false" ht="26.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="J10" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="K10" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="L10" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="26.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="K11" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="L11" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="26.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="K12" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="L12" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="26.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="K13" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="L13" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="26.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E14" s="7"/>
+      <c r="I14" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="J14" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="K14" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="L14" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" s="8" customFormat="true" ht="26.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="I15" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="J15" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="K15" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="L15" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="AMG15" s="4"/>
+      <c r="AMH15" s="4"/>
+      <c r="AMI15" s="4"/>
+      <c r="AMJ15" s="4"/>
+    </row>
+    <row r="16" customFormat="false" ht="26.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E16" s="7"/>
+      <c r="I16" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="J16" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="K16" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="L16" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" s="8" customFormat="true" ht="26.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="I17" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="J17" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="K17" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="L17" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="AMG17" s="4"/>
+      <c r="AMH17" s="4"/>
+      <c r="AMI17" s="4"/>
+      <c r="AMJ17" s="4"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>